<commit_message>
Journal of Ecology submission documents
</commit_message>
<xml_diff>
--- a/results/Supporting information/Table S2. Results models incubator as fixed factor.xlsx
+++ b/results/Supporting information/Table S2. Results models incubator as fixed factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Experiments/Move-along/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Germination_phenology/results/Supporting information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{116A4D7B-F860-481B-B206-15666673BD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F33CF6B4-48FE-404A-80EA-85C9A04B9967}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{116A4D7B-F860-481B-B206-15666673BD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BB0FEEC-01CB-4802-ACE5-6AA609E92D9D}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="0" windowWidth="17985" windowHeight="15540" xr2:uid="{42DE64D1-BFDA-4BCD-B96A-E1A04B27C6B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42DE64D1-BFDA-4BCD-B96A-E1A04B27C6B4}"/>
   </bookViews>
   <sheets>
     <sheet name="models fixed" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>incubatorSnowbed</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t xml:space="preserve"> germination trait ~ incubator   Random =    ~ animal +  code:ID</t>
+  </si>
+  <si>
+    <t>Table S2. Separate model results for each study system with incubator as fixed factor.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +118,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -479,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -493,6 +503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,15 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,6 +587,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -879,10 +890,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8611D42E-A5F3-4166-8BCE-0451B98038AB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:M18"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,48 +904,64 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+    </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="9" t="s">
         <v>13</v>
       </c>
@@ -964,13 +994,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="4">
         <v>0.32779999999999998</v>
       </c>
@@ -983,31 +1013,31 @@
       <c r="G5" s="3">
         <v>7623</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="11">
         <v>0.88800000000000001</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="4">
         <v>-5.4088000000000003</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="3">
         <v>-11.4717</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="3">
         <v>-0.29770000000000002</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="3">
         <v>1086</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="11">
         <v>3.3300000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="6">
         <v>-1.3129999999999999</v>
       </c>
@@ -1020,33 +1050,33 @@
       <c r="G6" s="5">
         <v>9000</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="6">
         <v>-2.8734000000000002</v>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="5">
         <v>-3.3730000000000002</v>
       </c>
-      <c r="K6" s="37">
+      <c r="K6" s="5">
         <v>-2.4062000000000001</v>
       </c>
-      <c r="L6" s="37">
+      <c r="L6" s="5">
         <v>7390</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="4">
         <v>-8.9130000000000003</v>
       </c>
@@ -1059,31 +1089,31 @@
       <c r="G7" s="3">
         <v>7967</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="11">
         <v>2.22E-4</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="4">
         <v>-13.352</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="3">
         <v>-18.925000000000001</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="3">
         <v>-7.9930000000000003</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="3">
         <v>896.8</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="6">
         <v>5.2750000000000004</v>
       </c>
@@ -1096,33 +1126,33 @@
       <c r="G8" s="5">
         <v>5012</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="6">
         <v>8.0269999999999992</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="5">
         <v>5.44</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="5">
         <v>10.831</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="5">
         <v>511.1</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="4">
         <v>-4.0134999999999996</v>
       </c>
@@ -1135,31 +1165,31 @@
       <c r="G9" s="3">
         <v>7764</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="11">
         <v>5.11E-2</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="4">
         <v>-2.2130000000000001</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="3">
         <v>-6.718</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="3">
         <v>2.4319999999999999</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="3">
         <v>7718</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="11">
         <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="29"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="6">
         <v>-1.482</v>
       </c>
@@ -1172,33 +1202,33 @@
       <c r="G10" s="5">
         <v>8625</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="6">
         <v>-3.2429999999999999</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="5">
         <v>-3.7669999999999999</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="5">
         <v>-2.7440000000000002</v>
       </c>
-      <c r="L10" s="37">
+      <c r="L10" s="5">
         <v>8676</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="4">
         <v>-6.18</v>
       </c>
@@ -1211,31 +1241,31 @@
       <c r="G11" s="3">
         <v>8387</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="11">
         <v>2E-3</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="4">
         <v>-4.601</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="3">
         <v>-7.1790000000000003</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="3">
         <v>-2.0939999999999999</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="3">
         <v>9000</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="11">
         <v>1.56E-3</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="6">
         <v>1.8939999999999999</v>
       </c>
@@ -1248,33 +1278,33 @@
       <c r="G12" s="5">
         <v>8683</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="6">
         <v>3.15</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="5">
         <v>2.6349999999999998</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="5">
         <v>3.65</v>
       </c>
-      <c r="L12" s="37">
+      <c r="L12" s="5">
         <v>9000</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="12">
         <v>1E-4</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="4">
         <v>4.3683300000000003</v>
       </c>
@@ -1287,31 +1317,31 @@
       <c r="G13" s="3">
         <v>7825</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="11">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="4">
         <v>2.0964999999999998</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="3">
         <v>-1.2157</v>
       </c>
-      <c r="K13" s="34">
+      <c r="K13" s="3">
         <v>5.0541</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="3">
         <v>9000</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M13" s="11">
         <v>0.16955999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="6">
         <v>-0.18778</v>
       </c>
@@ -1324,33 +1354,33 @@
       <c r="G14" s="5">
         <v>9042</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H14" s="12">
         <v>0.33579999999999999</v>
       </c>
-      <c r="I14" s="36">
+      <c r="I14" s="6">
         <v>-0.55010000000000003</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="5">
         <v>-0.88109999999999999</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="5">
         <v>-0.20669999999999999</v>
       </c>
-      <c r="L14" s="37">
+      <c r="L14" s="5">
         <v>9000</v>
       </c>
-      <c r="M14" s="35">
+      <c r="M14" s="12">
         <v>1.1100000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="4">
         <v>-1.6990000000000002E-2</v>
       </c>
@@ -1363,31 +1393,31 @@
       <c r="G15" s="3">
         <v>9000</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="11">
         <v>0.95199999999999996</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="4">
         <v>-0.35289999999999999</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="3">
         <v>-0.99280000000000002</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="3">
         <v>0.25979999999999998</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="3">
         <v>9000</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M15" s="11">
         <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="6">
         <v>0.33189999999999997</v>
       </c>
@@ -1400,33 +1430,33 @@
       <c r="G16" s="5">
         <v>9000</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="36">
+      <c r="I16" s="6">
         <v>0.82469999999999999</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="5">
         <v>0.64859999999999995</v>
       </c>
-      <c r="K16" s="37">
+      <c r="K16" s="5">
         <v>0.99109999999999998</v>
       </c>
-      <c r="L16" s="37">
+      <c r="L16" s="5">
         <v>9000</v>
       </c>
-      <c r="M16" s="35" t="s">
+      <c r="M16" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="4">
         <v>0.14607000000000001</v>
       </c>
@@ -1439,31 +1469,31 @@
       <c r="G17" s="3">
         <v>9000</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="11">
         <v>0.626</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="4">
         <v>6.6830000000000001E-2</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="3">
         <v>-0.57943</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="3">
         <v>0.74326999999999999</v>
       </c>
-      <c r="L17" s="34">
+      <c r="L17" s="3">
         <v>9000</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="11">
         <v>0.83799999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="30" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="2">
         <v>-0.16617999999999999</v>
       </c>
@@ -1476,27 +1506,28 @@
       <c r="G18" s="1">
         <v>9000</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="13">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="2">
         <v>0.13969999999999999</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="1">
         <v>-9.1980000000000006E-2</v>
       </c>
-      <c r="K18" s="40">
+      <c r="K18" s="1">
         <v>0.3599</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L18" s="1">
         <v>9000</v>
       </c>
-      <c r="M18" s="38">
+      <c r="M18" s="13">
         <v>0.216</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
+    <mergeCell ref="A1:M1"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -1525,6 +1556,6 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>